<commit_message>
redo the ngHO Calib
</commit_message>
<xml_diff>
--- a/ngHOcalib.xlsx
+++ b/ngHOcalib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amohamed/ownCloud/HO/generalMapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43478137-327F-0643-A5B3-7345D8872D2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639D02E4-A95E-4547-9123-F106C78BF4EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="20020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lmap_HOcalib" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="98">
   <si>
     <t>Side</t>
   </si>
@@ -291,6 +291,42 @@
   </si>
   <si>
     <t>dodeca</t>
+  </si>
+  <si>
+    <t>HO2M02</t>
+  </si>
+  <si>
+    <t>HO2M04</t>
+  </si>
+  <si>
+    <t>HO2M06</t>
+  </si>
+  <si>
+    <t>HO2M08</t>
+  </si>
+  <si>
+    <t>HO2M10</t>
+  </si>
+  <si>
+    <t>HO2M12</t>
+  </si>
+  <si>
+    <t>HO2P02</t>
+  </si>
+  <si>
+    <t>HO2P04</t>
+  </si>
+  <si>
+    <t>HO2P06</t>
+  </si>
+  <si>
+    <t>HO2P08</t>
+  </si>
+  <si>
+    <t>HO2P10</t>
+  </si>
+  <si>
+    <t>HO2P12</t>
   </si>
 </sst>
 </file>
@@ -763,12 +799,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="800" activePane="bottomLeft"/>
-      <selection sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="800" topLeftCell="A48" activePane="bottomLeft"/>
+      <selection activeCell="W1" sqref="W1"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53:W78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4483,6 +4519,1852 @@
         <v>999994</v>
       </c>
     </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>-1</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>71</v>
+      </c>
+      <c r="D53">
+        <v>12</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" t="s">
+        <v>86</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>47</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>5</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>1.5</v>
+      </c>
+      <c r="Q53">
+        <v>7</v>
+      </c>
+      <c r="R53">
+        <v>26</v>
+      </c>
+      <c r="S53">
+        <v>4</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+      <c r="U53">
+        <v>18</v>
+      </c>
+      <c r="V53">
+        <v>1129</v>
+      </c>
+      <c r="W53">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>-1</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>71</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" t="s">
+        <v>86</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>47</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>2</v>
+      </c>
+      <c r="M54">
+        <v>5</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="P54">
+        <v>1.5</v>
+      </c>
+      <c r="Q54">
+        <v>7</v>
+      </c>
+      <c r="R54">
+        <v>26</v>
+      </c>
+      <c r="S54">
+        <v>4</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <v>18</v>
+      </c>
+      <c r="V54">
+        <v>1128</v>
+      </c>
+      <c r="W54">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>-1</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>11</v>
+      </c>
+      <c r="D55">
+        <v>12</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" t="s">
+        <v>87</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>47</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>5</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>2.5</v>
+      </c>
+      <c r="Q55">
+        <v>8</v>
+      </c>
+      <c r="R55">
+        <v>26</v>
+      </c>
+      <c r="S55">
+        <v>4</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="U55">
+        <v>19</v>
+      </c>
+      <c r="V55">
+        <v>1128</v>
+      </c>
+      <c r="W55">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>-1</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>11</v>
+      </c>
+      <c r="D56">
+        <v>12</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>47</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+      <c r="M56">
+        <v>5</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>2.5</v>
+      </c>
+      <c r="Q56">
+        <v>8</v>
+      </c>
+      <c r="R56">
+        <v>26</v>
+      </c>
+      <c r="S56">
+        <v>4</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="U56">
+        <v>19</v>
+      </c>
+      <c r="V56">
+        <v>1128</v>
+      </c>
+      <c r="W56">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>-1</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>23</v>
+      </c>
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57">
+        <v>6</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>47</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>5</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>3.5</v>
+      </c>
+      <c r="Q57">
+        <v>9</v>
+      </c>
+      <c r="R57">
+        <v>26</v>
+      </c>
+      <c r="S57">
+        <v>4</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>20</v>
+      </c>
+      <c r="V57">
+        <v>1128</v>
+      </c>
+      <c r="W57">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>-1</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>23</v>
+      </c>
+      <c r="D58">
+        <v>12</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" t="s">
+        <v>88</v>
+      </c>
+      <c r="H58">
+        <v>6</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>47</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <v>5</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="P58">
+        <v>3.5</v>
+      </c>
+      <c r="Q58">
+        <v>9</v>
+      </c>
+      <c r="R58">
+        <v>26</v>
+      </c>
+      <c r="S58">
+        <v>4</v>
+      </c>
+      <c r="T58">
+        <v>1</v>
+      </c>
+      <c r="U58">
+        <v>20</v>
+      </c>
+      <c r="V58">
+        <v>1128</v>
+      </c>
+      <c r="W58">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>-1</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>35</v>
+      </c>
+      <c r="D59">
+        <v>12</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" t="s">
+        <v>89</v>
+      </c>
+      <c r="H59">
+        <v>8</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>47</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>5</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>4.5</v>
+      </c>
+      <c r="Q59">
+        <v>10</v>
+      </c>
+      <c r="R59">
+        <v>26</v>
+      </c>
+      <c r="S59">
+        <v>4</v>
+      </c>
+      <c r="T59">
+        <v>1</v>
+      </c>
+      <c r="U59">
+        <v>21</v>
+      </c>
+      <c r="V59">
+        <v>1128</v>
+      </c>
+      <c r="W59">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>-1</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>35</v>
+      </c>
+      <c r="D60">
+        <v>12</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" t="s">
+        <v>89</v>
+      </c>
+      <c r="H60">
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>47</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+      <c r="M60">
+        <v>5</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>4.5</v>
+      </c>
+      <c r="Q60">
+        <v>10</v>
+      </c>
+      <c r="R60">
+        <v>26</v>
+      </c>
+      <c r="S60">
+        <v>4</v>
+      </c>
+      <c r="T60">
+        <v>1</v>
+      </c>
+      <c r="U60">
+        <v>21</v>
+      </c>
+      <c r="V60">
+        <v>1128</v>
+      </c>
+      <c r="W60">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>-1</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>47</v>
+      </c>
+      <c r="D61">
+        <v>12</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
+        <v>90</v>
+      </c>
+      <c r="H61">
+        <v>10</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>47</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>5</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>5.5</v>
+      </c>
+      <c r="Q61">
+        <v>11</v>
+      </c>
+      <c r="R61">
+        <v>26</v>
+      </c>
+      <c r="S61">
+        <v>4</v>
+      </c>
+      <c r="T61">
+        <v>1</v>
+      </c>
+      <c r="U61">
+        <v>22</v>
+      </c>
+      <c r="V61">
+        <v>1128</v>
+      </c>
+      <c r="W61">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>-1</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>47</v>
+      </c>
+      <c r="D62">
+        <v>12</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" t="s">
+        <v>90</v>
+      </c>
+      <c r="H62">
+        <v>10</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62" t="s">
+        <v>47</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>2</v>
+      </c>
+      <c r="M62">
+        <v>5</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>5.5</v>
+      </c>
+      <c r="Q62">
+        <v>11</v>
+      </c>
+      <c r="R62">
+        <v>26</v>
+      </c>
+      <c r="S62">
+        <v>4</v>
+      </c>
+      <c r="T62">
+        <v>1</v>
+      </c>
+      <c r="U62">
+        <v>22</v>
+      </c>
+      <c r="V62">
+        <v>1128</v>
+      </c>
+      <c r="W62">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>-1</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>59</v>
+      </c>
+      <c r="D63">
+        <v>12</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" t="s">
+        <v>91</v>
+      </c>
+      <c r="H63">
+        <v>12</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63" t="s">
+        <v>47</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>5</v>
+      </c>
+      <c r="N63">
+        <v>1</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>6.5</v>
+      </c>
+      <c r="Q63">
+        <v>12</v>
+      </c>
+      <c r="R63">
+        <v>26</v>
+      </c>
+      <c r="S63">
+        <v>4</v>
+      </c>
+      <c r="T63">
+        <v>1</v>
+      </c>
+      <c r="U63">
+        <v>23</v>
+      </c>
+      <c r="V63">
+        <v>1128</v>
+      </c>
+      <c r="W63">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>-1</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>59</v>
+      </c>
+      <c r="D64">
+        <v>12</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" t="s">
+        <v>91</v>
+      </c>
+      <c r="H64">
+        <v>12</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>47</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>2</v>
+      </c>
+      <c r="M64">
+        <v>5</v>
+      </c>
+      <c r="N64">
+        <v>1</v>
+      </c>
+      <c r="O64">
+        <v>1</v>
+      </c>
+      <c r="P64">
+        <v>6.5</v>
+      </c>
+      <c r="Q64">
+        <v>12</v>
+      </c>
+      <c r="R64">
+        <v>26</v>
+      </c>
+      <c r="S64">
+        <v>4</v>
+      </c>
+      <c r="T64">
+        <v>1</v>
+      </c>
+      <c r="U64">
+        <v>23</v>
+      </c>
+      <c r="V64">
+        <v>1128</v>
+      </c>
+      <c r="W64">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>-1</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>59</v>
+      </c>
+      <c r="D65">
+        <v>12</v>
+      </c>
+      <c r="E65">
+        <v>7</v>
+      </c>
+      <c r="F65" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" t="s">
+        <v>91</v>
+      </c>
+      <c r="H65">
+        <v>12</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>47</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>3</v>
+      </c>
+      <c r="M65">
+        <v>5</v>
+      </c>
+      <c r="N65">
+        <v>1</v>
+      </c>
+      <c r="O65">
+        <v>2</v>
+      </c>
+      <c r="P65">
+        <v>6.5</v>
+      </c>
+      <c r="Q65">
+        <v>12</v>
+      </c>
+      <c r="R65">
+        <v>26</v>
+      </c>
+      <c r="S65">
+        <v>4</v>
+      </c>
+      <c r="T65">
+        <v>1</v>
+      </c>
+      <c r="U65">
+        <v>23</v>
+      </c>
+      <c r="V65">
+        <v>1128</v>
+      </c>
+      <c r="W65">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>71</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>14</v>
+      </c>
+      <c r="G66" t="s">
+        <v>92</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66" t="s">
+        <v>47</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <v>5</v>
+      </c>
+      <c r="N66">
+        <v>1</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>1.5</v>
+      </c>
+      <c r="Q66">
+        <v>7</v>
+      </c>
+      <c r="R66">
+        <v>27</v>
+      </c>
+      <c r="S66">
+        <v>4</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <v>18</v>
+      </c>
+      <c r="V66">
+        <v>1126</v>
+      </c>
+      <c r="W66">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>71</v>
+      </c>
+      <c r="D67">
+        <v>12</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>14</v>
+      </c>
+      <c r="G67" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>47</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>2</v>
+      </c>
+      <c r="M67">
+        <v>5</v>
+      </c>
+      <c r="N67">
+        <v>1</v>
+      </c>
+      <c r="O67">
+        <v>1</v>
+      </c>
+      <c r="P67">
+        <v>1.5</v>
+      </c>
+      <c r="Q67">
+        <v>7</v>
+      </c>
+      <c r="R67">
+        <v>27</v>
+      </c>
+      <c r="S67">
+        <v>4</v>
+      </c>
+      <c r="T67">
+        <v>1</v>
+      </c>
+      <c r="U67">
+        <v>18</v>
+      </c>
+      <c r="V67">
+        <v>1126</v>
+      </c>
+      <c r="W67">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>11</v>
+      </c>
+      <c r="D68">
+        <v>12</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>14</v>
+      </c>
+      <c r="G68" t="s">
+        <v>93</v>
+      </c>
+      <c r="H68">
+        <v>4</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>47</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>5</v>
+      </c>
+      <c r="N68">
+        <v>1</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>2.5</v>
+      </c>
+      <c r="Q68">
+        <v>8</v>
+      </c>
+      <c r="R68">
+        <v>27</v>
+      </c>
+      <c r="S68">
+        <v>4</v>
+      </c>
+      <c r="T68">
+        <v>1</v>
+      </c>
+      <c r="U68">
+        <v>19</v>
+      </c>
+      <c r="V68">
+        <v>1126</v>
+      </c>
+      <c r="W68">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69">
+        <v>11</v>
+      </c>
+      <c r="D69">
+        <v>12</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>14</v>
+      </c>
+      <c r="G69" t="s">
+        <v>93</v>
+      </c>
+      <c r="H69">
+        <v>4</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>47</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>2</v>
+      </c>
+      <c r="M69">
+        <v>5</v>
+      </c>
+      <c r="N69">
+        <v>1</v>
+      </c>
+      <c r="O69">
+        <v>1</v>
+      </c>
+      <c r="P69">
+        <v>2.5</v>
+      </c>
+      <c r="Q69">
+        <v>8</v>
+      </c>
+      <c r="R69">
+        <v>27</v>
+      </c>
+      <c r="S69">
+        <v>4</v>
+      </c>
+      <c r="T69">
+        <v>1</v>
+      </c>
+      <c r="U69">
+        <v>19</v>
+      </c>
+      <c r="V69">
+        <v>1126</v>
+      </c>
+      <c r="W69">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70">
+        <v>23</v>
+      </c>
+      <c r="D70">
+        <v>12</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" t="s">
+        <v>94</v>
+      </c>
+      <c r="H70">
+        <v>6</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>47</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <v>5</v>
+      </c>
+      <c r="N70">
+        <v>1</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>3.5</v>
+      </c>
+      <c r="Q70">
+        <v>9</v>
+      </c>
+      <c r="R70">
+        <v>27</v>
+      </c>
+      <c r="S70">
+        <v>4</v>
+      </c>
+      <c r="T70">
+        <v>1</v>
+      </c>
+      <c r="U70">
+        <v>20</v>
+      </c>
+      <c r="V70">
+        <v>1126</v>
+      </c>
+      <c r="W70">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>23</v>
+      </c>
+      <c r="D71">
+        <v>12</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" t="s">
+        <v>94</v>
+      </c>
+      <c r="H71">
+        <v>6</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>47</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>5</v>
+      </c>
+      <c r="N71">
+        <v>1</v>
+      </c>
+      <c r="O71">
+        <v>1</v>
+      </c>
+      <c r="P71">
+        <v>3.5</v>
+      </c>
+      <c r="Q71">
+        <v>9</v>
+      </c>
+      <c r="R71">
+        <v>27</v>
+      </c>
+      <c r="S71">
+        <v>4</v>
+      </c>
+      <c r="T71">
+        <v>1</v>
+      </c>
+      <c r="U71">
+        <v>20</v>
+      </c>
+      <c r="V71">
+        <v>1126</v>
+      </c>
+      <c r="W71">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <v>35</v>
+      </c>
+      <c r="D72">
+        <v>12</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" t="s">
+        <v>95</v>
+      </c>
+      <c r="H72">
+        <v>8</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>47</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72">
+        <v>5</v>
+      </c>
+      <c r="N72">
+        <v>1</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>4.5</v>
+      </c>
+      <c r="Q72">
+        <v>10</v>
+      </c>
+      <c r="R72">
+        <v>27</v>
+      </c>
+      <c r="S72">
+        <v>4</v>
+      </c>
+      <c r="T72">
+        <v>1</v>
+      </c>
+      <c r="U72">
+        <v>21</v>
+      </c>
+      <c r="V72">
+        <v>1126</v>
+      </c>
+      <c r="W72">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>35</v>
+      </c>
+      <c r="D73">
+        <v>12</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" t="s">
+        <v>95</v>
+      </c>
+      <c r="H73">
+        <v>8</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73" t="s">
+        <v>47</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>2</v>
+      </c>
+      <c r="M73">
+        <v>5</v>
+      </c>
+      <c r="N73">
+        <v>1</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <v>4.5</v>
+      </c>
+      <c r="Q73">
+        <v>10</v>
+      </c>
+      <c r="R73">
+        <v>27</v>
+      </c>
+      <c r="S73">
+        <v>4</v>
+      </c>
+      <c r="T73">
+        <v>1</v>
+      </c>
+      <c r="U73">
+        <v>21</v>
+      </c>
+      <c r="V73">
+        <v>1126</v>
+      </c>
+      <c r="W73">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>47</v>
+      </c>
+      <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>14</v>
+      </c>
+      <c r="G74" t="s">
+        <v>96</v>
+      </c>
+      <c r="H74">
+        <v>10</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74" t="s">
+        <v>47</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>5</v>
+      </c>
+      <c r="N74">
+        <v>1</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>5.5</v>
+      </c>
+      <c r="Q74">
+        <v>11</v>
+      </c>
+      <c r="R74">
+        <v>27</v>
+      </c>
+      <c r="S74">
+        <v>4</v>
+      </c>
+      <c r="T74">
+        <v>1</v>
+      </c>
+      <c r="U74">
+        <v>22</v>
+      </c>
+      <c r="V74">
+        <v>1126</v>
+      </c>
+      <c r="W74">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>47</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" t="s">
+        <v>96</v>
+      </c>
+      <c r="H75">
+        <v>10</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75" t="s">
+        <v>47</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>2</v>
+      </c>
+      <c r="M75">
+        <v>5</v>
+      </c>
+      <c r="N75">
+        <v>1</v>
+      </c>
+      <c r="O75">
+        <v>1</v>
+      </c>
+      <c r="P75">
+        <v>5.5</v>
+      </c>
+      <c r="Q75">
+        <v>11</v>
+      </c>
+      <c r="R75">
+        <v>27</v>
+      </c>
+      <c r="S75">
+        <v>4</v>
+      </c>
+      <c r="T75">
+        <v>1</v>
+      </c>
+      <c r="U75">
+        <v>22</v>
+      </c>
+      <c r="V75">
+        <v>1126</v>
+      </c>
+      <c r="W75">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76">
+        <v>47</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
+      </c>
+      <c r="E76">
+        <v>7</v>
+      </c>
+      <c r="F76" t="s">
+        <v>14</v>
+      </c>
+      <c r="G76" t="s">
+        <v>96</v>
+      </c>
+      <c r="H76">
+        <v>10</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>47</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>3</v>
+      </c>
+      <c r="M76">
+        <v>5</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+      <c r="O76">
+        <v>2</v>
+      </c>
+      <c r="P76">
+        <v>5.5</v>
+      </c>
+      <c r="Q76">
+        <v>11</v>
+      </c>
+      <c r="R76">
+        <v>27</v>
+      </c>
+      <c r="S76">
+        <v>4</v>
+      </c>
+      <c r="T76">
+        <v>1</v>
+      </c>
+      <c r="U76">
+        <v>22</v>
+      </c>
+      <c r="V76">
+        <v>1126</v>
+      </c>
+      <c r="W76">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77">
+        <v>59</v>
+      </c>
+      <c r="D77">
+        <v>12</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" t="s">
+        <v>97</v>
+      </c>
+      <c r="H77">
+        <v>12</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77" t="s">
+        <v>47</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>5</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>6.5</v>
+      </c>
+      <c r="Q77">
+        <v>12</v>
+      </c>
+      <c r="R77">
+        <v>27</v>
+      </c>
+      <c r="S77">
+        <v>4</v>
+      </c>
+      <c r="T77">
+        <v>1</v>
+      </c>
+      <c r="U77">
+        <v>23</v>
+      </c>
+      <c r="V77">
+        <v>1126</v>
+      </c>
+      <c r="W77">
+        <v>999994</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <v>59</v>
+      </c>
+      <c r="D78">
+        <v>12</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>14</v>
+      </c>
+      <c r="G78" t="s">
+        <v>97</v>
+      </c>
+      <c r="H78">
+        <v>12</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78" t="s">
+        <v>47</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>2</v>
+      </c>
+      <c r="M78">
+        <v>5</v>
+      </c>
+      <c r="N78">
+        <v>1</v>
+      </c>
+      <c r="O78">
+        <v>1</v>
+      </c>
+      <c r="P78">
+        <v>6.5</v>
+      </c>
+      <c r="Q78">
+        <v>12</v>
+      </c>
+      <c r="R78">
+        <v>27</v>
+      </c>
+      <c r="S78">
+        <v>4</v>
+      </c>
+      <c r="T78">
+        <v>1</v>
+      </c>
+      <c r="U78">
+        <v>23</v>
+      </c>
+      <c r="V78">
+        <v>1126</v>
+      </c>
+      <c r="W78">
+        <v>999994</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W52">
     <sortCondition ref="S2:S52"/>
@@ -4498,12 +6380,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93411F5-6A9D-D844-BEBB-FDC048972878}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="800" activePane="bottomLeft"/>
       <selection sqref="A1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="M72" sqref="M72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6493,6 +8375,994 @@
         <v>1</v>
       </c>
     </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53">
+        <v>26</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>84</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>18</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <v>-2</v>
+      </c>
+      <c r="K53">
+        <v>71</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54">
+        <v>26</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>18</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54">
+        <v>-2</v>
+      </c>
+      <c r="K54">
+        <v>71</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55">
+        <v>26</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
+      <c r="G55">
+        <v>19</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55">
+        <v>-2</v>
+      </c>
+      <c r="K55">
+        <v>11</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56">
+        <v>26</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>84</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>8</v>
+      </c>
+      <c r="G56">
+        <v>19</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56">
+        <v>-2</v>
+      </c>
+      <c r="K56">
+        <v>11</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>9</v>
+      </c>
+      <c r="G57">
+        <v>20</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57">
+        <v>-2</v>
+      </c>
+      <c r="K57">
+        <v>23</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58">
+        <v>26</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>9</v>
+      </c>
+      <c r="G58">
+        <v>20</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58">
+        <v>-2</v>
+      </c>
+      <c r="K58">
+        <v>23</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>84</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>10</v>
+      </c>
+      <c r="G59">
+        <v>21</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59">
+        <v>-2</v>
+      </c>
+      <c r="K59">
+        <v>35</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60">
+        <v>26</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>10</v>
+      </c>
+      <c r="G60">
+        <v>21</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60">
+        <v>-2</v>
+      </c>
+      <c r="K60">
+        <v>35</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>83</v>
+      </c>
+      <c r="B61">
+        <v>26</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>84</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>11</v>
+      </c>
+      <c r="G61">
+        <v>22</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61">
+        <v>-2</v>
+      </c>
+      <c r="K61">
+        <v>47</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62">
+        <v>26</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>11</v>
+      </c>
+      <c r="G62">
+        <v>22</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62">
+        <v>-2</v>
+      </c>
+      <c r="K62">
+        <v>47</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63">
+        <v>26</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>12</v>
+      </c>
+      <c r="G63">
+        <v>23</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>14</v>
+      </c>
+      <c r="J63">
+        <v>-2</v>
+      </c>
+      <c r="K63">
+        <v>59</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64">
+        <v>26</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>84</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>12</v>
+      </c>
+      <c r="G64">
+        <v>23</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64">
+        <v>-2</v>
+      </c>
+      <c r="K64">
+        <v>59</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65">
+        <v>26</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>12</v>
+      </c>
+      <c r="G65">
+        <v>23</v>
+      </c>
+      <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="I65" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65">
+        <v>-2</v>
+      </c>
+      <c r="K65">
+        <v>59</v>
+      </c>
+      <c r="L65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66">
+        <v>27</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>84</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>7</v>
+      </c>
+      <c r="G66">
+        <v>18</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66">
+        <v>2</v>
+      </c>
+      <c r="K66">
+        <v>71</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67">
+        <v>27</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>7</v>
+      </c>
+      <c r="G67">
+        <v>18</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67" t="s">
+        <v>14</v>
+      </c>
+      <c r="J67">
+        <v>2</v>
+      </c>
+      <c r="K67">
+        <v>71</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>83</v>
+      </c>
+      <c r="B68">
+        <v>27</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>84</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>8</v>
+      </c>
+      <c r="G68">
+        <v>19</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
+        <v>14</v>
+      </c>
+      <c r="J68">
+        <v>2</v>
+      </c>
+      <c r="K68">
+        <v>11</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69">
+        <v>27</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>8</v>
+      </c>
+      <c r="G69">
+        <v>19</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69" t="s">
+        <v>14</v>
+      </c>
+      <c r="J69">
+        <v>2</v>
+      </c>
+      <c r="K69">
+        <v>11</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70">
+        <v>27</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>84</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>9</v>
+      </c>
+      <c r="G70">
+        <v>20</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>14</v>
+      </c>
+      <c r="J70">
+        <v>2</v>
+      </c>
+      <c r="K70">
+        <v>23</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71">
+        <v>27</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>84</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>9</v>
+      </c>
+      <c r="G71">
+        <v>20</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71" t="s">
+        <v>14</v>
+      </c>
+      <c r="J71">
+        <v>2</v>
+      </c>
+      <c r="K71">
+        <v>23</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72">
+        <v>27</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>84</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>10</v>
+      </c>
+      <c r="G72">
+        <v>21</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" t="s">
+        <v>14</v>
+      </c>
+      <c r="J72">
+        <v>2</v>
+      </c>
+      <c r="K72">
+        <v>35</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73">
+        <v>27</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>84</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>10</v>
+      </c>
+      <c r="G73">
+        <v>21</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73">
+        <v>2</v>
+      </c>
+      <c r="K73">
+        <v>35</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74">
+        <v>27</v>
+      </c>
+      <c r="C74">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>84</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>11</v>
+      </c>
+      <c r="G74">
+        <v>22</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74" t="s">
+        <v>14</v>
+      </c>
+      <c r="J74">
+        <v>2</v>
+      </c>
+      <c r="K74">
+        <v>47</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>83</v>
+      </c>
+      <c r="B75">
+        <v>27</v>
+      </c>
+      <c r="C75">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>84</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>11</v>
+      </c>
+      <c r="G75">
+        <v>22</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75" t="s">
+        <v>14</v>
+      </c>
+      <c r="J75">
+        <v>2</v>
+      </c>
+      <c r="K75">
+        <v>47</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76">
+        <v>27</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>84</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>11</v>
+      </c>
+      <c r="G76">
+        <v>22</v>
+      </c>
+      <c r="H76">
+        <v>2</v>
+      </c>
+      <c r="I76" t="s">
+        <v>14</v>
+      </c>
+      <c r="J76">
+        <v>2</v>
+      </c>
+      <c r="K76">
+        <v>47</v>
+      </c>
+      <c r="L76">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77">
+        <v>27</v>
+      </c>
+      <c r="C77">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>84</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>12</v>
+      </c>
+      <c r="G77">
+        <v>23</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77">
+        <v>2</v>
+      </c>
+      <c r="K77">
+        <v>59</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78">
+        <v>27</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>84</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>12</v>
+      </c>
+      <c r="G78">
+        <v>23</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78" t="s">
+        <v>14</v>
+      </c>
+      <c r="J78">
+        <v>2</v>
+      </c>
+      <c r="K78">
+        <v>59</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="8" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>